<commit_message>
Castati tutti i messaggi di errore null a varchar(20) e aggiornate le pt
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/57_Inst_Customer_Unit_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/57_Inst_Customer_Unit_RETAIL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -170,9 +170,6 @@
     <t>Source_tableName</t>
   </si>
   <si>
-    <t>TEWSA0W</t>
-  </si>
-  <si>
     <t>IT_RETAIL</t>
   </si>
   <si>
@@ -192,12 +189,15 @@
   </si>
   <si>
     <t>RE_CUSTOMER_TABLE</t>
+  </si>
+  <si>
+    <t>TEWSA0D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -786,113 +786,22 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -900,7 +809,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="8953500" cy="9705975"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -925,6 +834,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -940,7 +897,50 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -988,7 +988,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1036,7 +1036,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1044,7 +1044,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9772650" cy="9525000"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1084,7 +1084,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1132,7 +1132,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1140,7 +1140,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9953625" cy="9525000"/>
+          <a:ext cx="9772650" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1180,7 +1180,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1228,7 +1228,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1271,6 +1271,54 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9953625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -1285,6 +1333,54 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10182225" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11268075" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1388,6 +1484,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1423,6 +1536,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1602,7 +1732,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,22 +1800,22 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1746,19 +1876,19 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>